<commit_message>
update training config and result
</commit_message>
<xml_diff>
--- a/HW1/Programming/Training Result.xlsx
+++ b/HW1/Programming/Training Result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NTU\First Year\Machine Learning\HW\HW1\Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E93D46B-0679-45A6-8334-B293B145FF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917DED57-73E5-466D-A896-2110BC16A9D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5265" yWindow="4185" windowWidth="21600" windowHeight="11295" tabRatio="404" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6915" yWindow="2970" windowWidth="12210" windowHeight="11295" tabRatio="404" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NTU_ML" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="21">
   <si>
     <t>Time</t>
   </si>
@@ -68,6 +68,22 @@
   </si>
   <si>
     <t>[0,5,7-13]</t>
+  </si>
+  <si>
+    <t>Use filter data function
+Normalization</t>
+  </si>
+  <si>
+    <t>6.05973(Invalid)</t>
+  </si>
+  <si>
+    <t>Did not normalize the testing data</t>
+  </si>
+  <si>
+    <t>[1-9, 13, 14]</t>
+  </si>
+  <si>
+    <t>[1-4, 6-9, 13, 14]</t>
   </si>
 </sst>
 </file>
@@ -367,10 +383,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -386,7 +402,7 @@
     <col min="10" max="16384" width="12.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -418,7 +434,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>44840</v>
       </c>
@@ -447,7 +463,7 @@
         <v>4.3551299999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>44840</v>
       </c>
@@ -476,7 +492,7 @@
         <v>6.2729999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>44840</v>
       </c>
@@ -505,7 +521,7 @@
         <v>4.6481399999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>44841</v>
       </c>
@@ -537,7 +553,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>44841</v>
       </c>
@@ -566,7 +582,7 @@
         <v>4.7484299999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>44841</v>
       </c>
@@ -598,50 +614,132 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>44841</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1">
+        <v>200</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="1">
+        <v>512</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>44842</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1">
+        <v>200</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="1">
+        <v>512</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="1">
+        <v>8.1476699999999997</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>44843</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1">
+        <v>100</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="1">
+        <v>512</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="1">
+        <v>3.9284699999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>44843</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1">
+        <v>100</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="1">
+        <v>512</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="1">
+        <v>3.79697</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -652,7 +750,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -663,7 +761,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -674,7 +772,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -685,7 +783,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -696,7 +794,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -705,7 +803,7 @@
       <c r="F17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -716,7 +814,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -727,7 +825,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -737,7 +835,7 @@
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -747,7 +845,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -757,7 +855,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -767,7 +865,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="1"/>
       <c r="C24" s="5"/>
@@ -778,7 +876,7 @@
       <c r="H24" s="5"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -789,7 +887,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -800,7 +898,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -811,7 +909,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -822,7 +920,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -833,7 +931,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -844,7 +942,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -855,7 +953,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -866,7 +964,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -877,7 +975,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -888,7 +986,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -899,7 +997,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -910,7 +1008,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -921,7 +1019,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -932,7 +1030,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -943,7 +1041,7 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -954,7 +1052,7 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>

</xml_diff>

<commit_message>
udpate training config and result
</commit_message>
<xml_diff>
--- a/HW1/Programming/Training Result.xlsx
+++ b/HW1/Programming/Training Result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NTU\First Year\Machine Learning\HW\HW1\Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917DED57-73E5-466D-A896-2110BC16A9D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF4ACE5-DF81-4D8E-BAAF-16F64845C9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6915" yWindow="2970" windowWidth="12210" windowHeight="11295" tabRatio="404" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9795" yWindow="1185" windowWidth="12210" windowHeight="11295" tabRatio="404" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NTU_ML" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="22">
   <si>
     <t>Time</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>[1-4, 6-9, 13, 14]</t>
+  </si>
+  <si>
+    <t>best weight &amp; best bias</t>
   </si>
 </sst>
 </file>
@@ -128,7 +131,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -145,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -160,6 +163,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -386,7 +392,7 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -709,6 +715,9 @@
       <c r="I10" s="1">
         <v>3.9284699999999999</v>
       </c>
+      <c r="J10" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
@@ -738,28 +747,73 @@
       <c r="I11" s="1">
         <v>3.79697</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="J11" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>44843</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1">
+        <v>100</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="1">
+        <v>512</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="7">
+        <v>3.2701099999999999</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>44843</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="1">
+        <v>512</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="1">
+        <v>4.3634500000000003</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>

</xml_diff>

<commit_message>
update training config & result
</commit_message>
<xml_diff>
--- a/HW1/Programming/Training Result.xlsx
+++ b/HW1/Programming/Training Result.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NTU\First Year\Machine Learning\HW\HW1\Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCACA4D0-F111-4581-B950-1D71661F7DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E42411-9F0C-4934-B341-24E646CFFE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11340" yWindow="1830" windowWidth="12210" windowHeight="11295" tabRatio="404" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11160" yWindow="1830" windowWidth="8145" windowHeight="11295" tabRatio="404" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NTU_ML" sheetId="1" r:id="rId1"/>
+    <sheet name="temp" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
   <si>
     <t>Time</t>
   </si>
@@ -99,6 +100,18 @@
   </si>
   <si>
     <t>MSE</t>
+  </si>
+  <si>
+    <t>Use filter data fucntion</t>
+  </si>
+  <si>
+    <t>Normalization</t>
+  </si>
+  <si>
+    <t>Unuse Normalization</t>
+  </si>
+  <si>
+    <t>Not use 2nd-order polynomial on testing</t>
   </si>
 </sst>
 </file>
@@ -108,7 +121,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -132,8 +145,14 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,6 +171,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -165,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -203,13 +228,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -432,8 +478,8 @@
   </sheetPr>
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -486,19 +532,19 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="14">
+      <c r="A2" s="17">
         <v>44840</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="15" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="8">
         <v>200</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="18">
         <v>0.1</v>
       </c>
       <c r="F2" s="8" t="s">
@@ -507,10 +553,10 @@
       <c r="G2" s="8">
         <v>512</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="15" t="s">
         <v>10</v>
       </c>
       <c r="J2" s="8">
@@ -518,55 +564,55 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
-      <c r="B3" s="12"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="8">
         <v>500</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="12" t="s">
+      <c r="D3" s="15"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="8">
         <v>1025</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
       <c r="J3" s="8">
         <v>6.2729999999999997</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12">
+      <c r="A4" s="17"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15">
         <v>200</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12">
+      <c r="D4" s="15"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15">
         <v>512</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
       <c r="J4" s="8">
         <v>4.6481399999999997</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="14">
+      <c r="A5" s="17">
         <v>44841</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
       <c r="J5" s="8">
         <v>5.9770500000000002</v>
       </c>
@@ -575,33 +621,33 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="13"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="18"/>
       <c r="F6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
       <c r="J6" s="8">
         <v>4.7484299999999999</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="12" t="s">
+      <c r="A7" s="17"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
       <c r="J7" s="1">
         <v>4.1391799999999996</v>
       </c>
@@ -610,15 +656,15 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
       <c r="J8" s="8" t="s">
         <v>16</v>
       </c>
@@ -633,14 +679,14 @@
       <c r="A9" s="7">
         <v>44842</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
       <c r="J9" s="8">
         <v>8.1476699999999997</v>
       </c>
@@ -649,74 +695,74 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="14">
+      <c r="A10" s="17">
         <v>44843</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12">
+      <c r="B10" s="15"/>
+      <c r="C10" s="15">
         <v>100</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="18"/>
       <c r="F10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
       <c r="J10" s="8">
         <v>3.9284699999999999</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="K10" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="12" t="s">
+      <c r="A11" s="17"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
       <c r="J11" s="8">
         <v>3.79697</v>
       </c>
-      <c r="K11" s="11"/>
+      <c r="K11" s="16"/>
     </row>
     <row r="12" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
       <c r="J12" s="1">
         <v>3.2701099999999999</v>
       </c>
-      <c r="K12" s="11"/>
+      <c r="K12" s="16"/>
     </row>
     <row r="13" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="8">
         <v>1000</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
       <c r="J13" s="8">
         <v>4.3634500000000003</v>
       </c>
@@ -725,121 +771,132 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="14">
+      <c r="A14" s="17">
         <v>44844</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="15">
         <v>100</v>
       </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
       <c r="J14" s="1">
         <v>3.29244</v>
       </c>
-      <c r="K14" s="11" t="s">
+      <c r="K14" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
       <c r="J15" s="6">
         <v>3.1390600000000002</v>
       </c>
-      <c r="K15" s="11"/>
+      <c r="K15" s="16"/>
     </row>
     <row r="16" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="14">
+      <c r="A16" s="13">
         <v>44845</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12">
+      <c r="B16" s="15"/>
+      <c r="C16" s="15">
         <v>10</v>
       </c>
-      <c r="D16" s="12"/>
+      <c r="D16" s="15"/>
       <c r="E16" s="10">
         <v>0.5</v>
       </c>
-      <c r="F16" s="12"/>
+      <c r="F16" s="15"/>
       <c r="G16" s="8">
         <v>256</v>
       </c>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
       <c r="J16" s="8">
         <v>3.4877099999999999</v>
       </c>
-      <c r="K16" s="11" t="s">
+      <c r="K16" s="16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="15">
+    <row r="17" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="17">
+        <v>44846</v>
+      </c>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="14">
         <v>0.2</v>
       </c>
-      <c r="F17" s="12"/>
+      <c r="F17" s="15"/>
       <c r="G17" s="3">
         <v>128</v>
       </c>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
       <c r="J17" s="4"/>
-      <c r="K17" s="11"/>
-    </row>
-    <row r="18" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="14"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="3">
+      <c r="K17" s="16"/>
+    </row>
+    <row r="18" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="17"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="19">
         <v>1000</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="20">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="F18" s="12"/>
-      <c r="G18" s="3">
+      <c r="F18" s="15"/>
+      <c r="G18" s="19">
         <v>1024</v>
       </c>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
       <c r="J18" s="9">
         <v>3.2196099999999999</v>
       </c>
-      <c r="K18" s="11"/>
-    </row>
-    <row r="19" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K18" s="16"/>
+      <c r="L18" s="16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="17"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="21">
+        <v>3.92536</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L19" s="16"/>
+    </row>
+    <row r="20" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -851,7 +908,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -863,7 +920,7 @@
       <c r="I21" s="3"/>
       <c r="J21" s="4"/>
     </row>
-    <row r="22" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -875,7 +932,7 @@
       <c r="I22" s="3"/>
       <c r="J22" s="4"/>
     </row>
-    <row r="23" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -887,7 +944,7 @@
       <c r="I23" s="3"/>
       <c r="J23" s="4"/>
     </row>
-    <row r="24" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="3"/>
       <c r="C24" s="5"/>
@@ -899,7 +956,7 @@
       <c r="I24" s="5"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -911,7 +968,7 @@
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -923,7 +980,7 @@
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -935,7 +992,7 @@
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -947,7 +1004,7 @@
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
     </row>
-    <row r="29" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="7"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -959,7 +1016,7 @@
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
     </row>
-    <row r="30" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="7"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -971,7 +1028,7 @@
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
     </row>
-    <row r="31" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="7"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -983,7 +1040,7 @@
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
     </row>
-    <row r="32" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -1104,14 +1161,25 @@
       <c r="J41" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="I2:I18"/>
+  <mergeCells count="27">
+    <mergeCell ref="I2:I19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F11:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H2:H19"/>
+    <mergeCell ref="E2:E15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="G4:G15"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="F3:F5"/>
     <mergeCell ref="K16:K18"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="D2:D17"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="F11:F18"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A8"/>
     <mergeCell ref="A10:A13"/>
@@ -1121,15 +1189,116 @@
     <mergeCell ref="K10:K12"/>
     <mergeCell ref="C4:C9"/>
     <mergeCell ref="C10:C12"/>
-    <mergeCell ref="E2:E15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="G4:G15"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="H2:H18"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A145EA25-B4E0-4AB0-AD79-9F83F44F4055}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="11" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="11">
+        <v>1000</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="11">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="11">
+        <v>1024</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="22">
+        <v>3.2196099999999999</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="11">
+        <v>1000</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="11">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="11">
+        <v>1024</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="22">
+        <v>3.92536</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update all report file
</commit_message>
<xml_diff>
--- a/HW1/Programming/Training Result.xlsx
+++ b/HW1/Programming/Training Result.xlsx
@@ -1,28 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NTU\First Year\Machine Learning\HW\HW1\Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2AD01E-D444-4FDF-B997-7756E0F9920E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDAFCF7-2A0E-4D47-92ED-E9C4A14AB773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11160" yWindow="1830" windowWidth="8145" windowHeight="11295" tabRatio="404" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="404" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NTU_ML" sheetId="1" r:id="rId1"/>
     <sheet name="temp" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="34">
   <si>
     <t>Time</t>
   </si>
@@ -113,6 +112,18 @@
   </si>
   <si>
     <t>RMSE(Lower is Better)</t>
+  </si>
+  <si>
+    <t>Filter Data</t>
+  </si>
+  <si>
+    <t>Norm. Data</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -147,7 +158,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,6 +183,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -185,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -235,31 +258,52 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -483,7 +527,7 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -536,7 +580,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="20">
+      <c r="A2" s="24">
         <v>44840</v>
       </c>
       <c r="B2" s="19" t="s">
@@ -548,7 +592,7 @@
       <c r="D2" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="20">
         <v>0.1</v>
       </c>
       <c r="F2" s="9" t="s">
@@ -570,13 +614,13 @@
       <c r="L2" s="11"/>
     </row>
     <row r="3" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="20"/>
+      <c r="A3" s="24"/>
       <c r="B3" s="19"/>
       <c r="C3" s="9">
         <v>500</v>
       </c>
       <c r="D3" s="19"/>
-      <c r="E3" s="23"/>
+      <c r="E3" s="20"/>
       <c r="F3" s="19" t="s">
         <v>10</v>
       </c>
@@ -592,13 +636,13 @@
       <c r="L3" s="11"/>
     </row>
     <row r="4" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="20"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="19"/>
       <c r="C4" s="19">
         <v>200</v>
       </c>
       <c r="D4" s="19"/>
-      <c r="E4" s="23"/>
+      <c r="E4" s="20"/>
       <c r="F4" s="19"/>
       <c r="G4" s="19">
         <v>512</v>
@@ -612,13 +656,13 @@
       <c r="L4" s="11"/>
     </row>
     <row r="5" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="20">
+      <c r="A5" s="24">
         <v>44841</v>
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
-      <c r="E5" s="23"/>
+      <c r="E5" s="20"/>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
@@ -632,11 +676,11 @@
       <c r="L5" s="11"/>
     </row>
     <row r="6" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="20"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
-      <c r="E6" s="23"/>
+      <c r="E6" s="20"/>
       <c r="F6" s="9" t="s">
         <v>13</v>
       </c>
@@ -650,11 +694,11 @@
       <c r="L6" s="11"/>
     </row>
     <row r="7" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="20"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
-      <c r="E7" s="23"/>
+      <c r="E7" s="20"/>
       <c r="F7" s="19" t="s">
         <v>7</v>
       </c>
@@ -670,11 +714,11 @@
       <c r="L7" s="11"/>
     </row>
     <row r="8" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="20"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
-      <c r="E8" s="23"/>
+      <c r="E8" s="20"/>
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
       <c r="H8" s="19"/>
@@ -696,7 +740,7 @@
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
-      <c r="E9" s="23"/>
+      <c r="E9" s="20"/>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
       <c r="H9" s="19"/>
@@ -710,7 +754,7 @@
       <c r="L9" s="11"/>
     </row>
     <row r="10" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="20">
+      <c r="A10" s="24">
         <v>44843</v>
       </c>
       <c r="B10" s="19"/>
@@ -718,7 +762,7 @@
         <v>100</v>
       </c>
       <c r="D10" s="19"/>
-      <c r="E10" s="23"/>
+      <c r="E10" s="20"/>
       <c r="F10" s="9" t="s">
         <v>17</v>
       </c>
@@ -734,11 +778,11 @@
       <c r="L10" s="11"/>
     </row>
     <row r="11" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="20"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
-      <c r="E11" s="23"/>
+      <c r="E11" s="20"/>
       <c r="F11" s="19" t="s">
         <v>18</v>
       </c>
@@ -752,11 +796,11 @@
       <c r="L11" s="11"/>
     </row>
     <row r="12" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="20"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
-      <c r="E12" s="23"/>
+      <c r="E12" s="20"/>
       <c r="F12" s="19"/>
       <c r="G12" s="19"/>
       <c r="H12" s="19"/>
@@ -768,7 +812,7 @@
       <c r="L12" s="11"/>
     </row>
     <row r="13" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="20"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="9" t="s">
         <v>19</v>
       </c>
@@ -776,7 +820,7 @@
         <v>1000</v>
       </c>
       <c r="D13" s="19"/>
-      <c r="E13" s="23"/>
+      <c r="E13" s="20"/>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
       <c r="H13" s="19"/>
@@ -790,7 +834,7 @@
       <c r="L13" s="11"/>
     </row>
     <row r="14" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="20">
+      <c r="A14" s="24">
         <v>44844</v>
       </c>
       <c r="B14" s="19" t="s">
@@ -800,7 +844,7 @@
         <v>100</v>
       </c>
       <c r="D14" s="19"/>
-      <c r="E14" s="23"/>
+      <c r="E14" s="20"/>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
       <c r="H14" s="19"/>
@@ -814,11 +858,11 @@
       <c r="L14" s="11"/>
     </row>
     <row r="15" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="20"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="19"/>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
-      <c r="E15" s="23"/>
+      <c r="E15" s="20"/>
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
@@ -856,7 +900,7 @@
       <c r="L16" s="11"/>
     </row>
     <row r="17" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="20">
+      <c r="A17" s="24">
         <v>44846</v>
       </c>
       <c r="B17" s="19"/>
@@ -876,7 +920,7 @@
       <c r="L17" s="11"/>
     </row>
     <row r="18" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="20"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="19"/>
       <c r="C18" s="21">
         <v>1000</v>
@@ -902,7 +946,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="20"/>
+      <c r="A19" s="24"/>
       <c r="B19" s="19"/>
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
@@ -944,20 +988,20 @@
       <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
     </row>
     <row r="23" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
@@ -1064,7 +1108,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>44848</v>
       </c>
@@ -1092,9 +1136,11 @@
       <c r="I26" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J26" s="7"/>
+      <c r="J26" s="7">
+        <v>2.4980099999999998</v>
+      </c>
       <c r="K26" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
@@ -1279,18 +1325,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="K16:K18"/>
-    <mergeCell ref="H2:H19"/>
-    <mergeCell ref="E2:E15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="G4:G15"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F11:F19"/>
-    <mergeCell ref="G18:G19"/>
     <mergeCell ref="A22:L22"/>
     <mergeCell ref="K14:K15"/>
     <mergeCell ref="K10:K12"/>
@@ -1307,6 +1341,18 @@
     <mergeCell ref="L18:L19"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="B14:B19"/>
+    <mergeCell ref="K16:K18"/>
+    <mergeCell ref="H2:H19"/>
+    <mergeCell ref="E2:E15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="G4:G15"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F11:F19"/>
+    <mergeCell ref="G18:G19"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1316,23 +1362,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A145EA25-B4E0-4AB0-AD79-9F83F44F4055}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView zoomScale="138" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="B1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="24"/>
-    <col min="2" max="2" width="11" style="24" customWidth="1"/>
-    <col min="3" max="7" width="9.140625" style="24"/>
-    <col min="8" max="8" width="12.42578125" style="24" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" style="24" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="24"/>
+    <col min="1" max="1" width="9.140625" style="5"/>
+    <col min="2" max="2" width="11" style="5" customWidth="1"/>
+    <col min="3" max="7" width="9.140625" style="5"/>
+    <col min="8" max="8" width="12.42578125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1358,68 +1404,143 @@
         <v>29</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>200</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="31">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="32">
         <v>1024</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="27">
         <v>2.4462299999999999</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I2" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>200</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="8">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="3">
-        <v>1024</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="B3" s="30"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
       <c r="H3" s="16">
         <v>2.13897</v>
       </c>
-      <c r="I3" s="25" t="s">
-        <v>12</v>
+      <c r="I3" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+    </row>
+    <row r="5" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
+        <v>100</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="31">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="32">
+        <v>512</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="26">
+        <v>2.4980099999999998</v>
+      </c>
+      <c r="I5" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
+        <v>100</v>
+      </c>
+      <c r="B6" s="30"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="25">
+        <v>2.1341100000000002</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>